<commit_message>
change hour time format in excel
</commit_message>
<xml_diff>
--- a/data/slot_history.xlsx
+++ b/data/slot_history.xlsx
@@ -423,11 +423,11 @@
       <c r="A2" t="str">
         <v>26/10 Sunday</v>
       </c>
-      <c r="B2">
-        <v>19.5</v>
-      </c>
-      <c r="C2">
-        <v>21</v>
+      <c r="B2" t="str">
+        <v>19:30</v>
+      </c>
+      <c r="C2" t="str">
+        <v>21:00</v>
       </c>
       <c r="D2" t="str">
         <v>2025-10-12 15:22</v>

</xml_diff>